<commit_message>
Revisión Guías PAUA Usuarios
</commit_message>
<xml_diff>
--- a/PAUA/ENTREGABLES/Matiz de Pruebas Login.xlsx
+++ b/PAUA/ENTREGABLES/Matiz de Pruebas Login.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INAP-QA\Documents\GITHUB\All-documents-\LOGIN\ENTREGABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\PAUA\ENTREGABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="101">
   <si>
     <t xml:space="preserve">Tester: Iris Lechuga </t>
   </si>
@@ -202,9 +202,6 @@
     <t>Abelino Olguín</t>
   </si>
   <si>
-    <t xml:space="preserve">Eliminación Correcta </t>
-  </si>
-  <si>
     <t>Jose Angel Pérez</t>
   </si>
   <si>
@@ -250,19 +247,7 @@
     <t xml:space="preserve">Muestra Mensaje de Notificación </t>
   </si>
   <si>
-    <t>Menú Incicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inicio </t>
-  </si>
-  <si>
-    <t>Despliega Submenús</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recibir notificaciones </t>
-  </si>
-  <si>
-    <t>Despliegue</t>
   </si>
   <si>
     <t>Mostrar la lista organizada que resume la información que se encuentra  dentro de la plataforma.</t>
@@ -274,154 +259,16 @@
     <t>Inicio</t>
   </si>
   <si>
-    <t xml:space="preserve">Muestra la introducción </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Engloba las acciones del usuario usara  en la plataforma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Financiamiento y Obligaciones </t>
-  </si>
-  <si>
-    <t>Crédito simple corto plazo</t>
-  </si>
-  <si>
-    <t>Correcto desglose</t>
-  </si>
-  <si>
     <t xml:space="preserve">Desglosa las submenús </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crédito Simple Corto Plazo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Encabezado </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Información General </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condiciones Financieras </t>
-  </si>
-  <si>
-    <t>Resumen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muestra información del usuario en sesión. </t>
-  </si>
-  <si>
-    <t>Se visualiza la información correspondiente al usuario (delalle en el temaño de fuente) - "Solicitante Autorizado"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apartado donde se agregan las condiciones financieras </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permite Agregar y Eliminar Registros </t>
   </si>
   <si>
     <t>Disposición / Pagos de Capital</t>
   </si>
   <si>
-    <t>Comisiones / Tasa efectiva</t>
-  </si>
-  <si>
-    <t>Documentación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulta de solicitudes </t>
-  </si>
-  <si>
-    <t>Consulta de solicitudes</t>
-  </si>
-  <si>
-    <t>Ver</t>
-  </si>
-  <si>
     <t xml:space="preserve">Editar  </t>
   </si>
   <si>
-    <t>Comentarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agregar Datos correspondientes y agregar registro en la tabla </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permite cargar y arrastrar documentos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documentación Eliminar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar los documentos “no obligatorios” </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Permite visualizar el estado de la solicitud como datos capturados y faltantes por capturar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solicitud de inscripción </t>
-  </si>
-  <si>
-    <t>Visualización de la información extraida de los campos anteriores.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancelar </t>
-  </si>
-  <si>
-    <t>Solicitar Modificación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardar Borrador </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finalizar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check list Selección Reglas </t>
-  </si>
-  <si>
-    <t>Selección al dar clic en el cuadro de check list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selección Correcta </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancela el registro </t>
-  </si>
-  <si>
-    <t>Cancelación Correcta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asignar Mensaje de modificacíón </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guardar registros como Borrador </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finaliza la solicitud se podrás ver visualizada en el apartado de  "Consulta de Solicitudes" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulta de Solicitudes </t>
-  </si>
-  <si>
-    <t>Borrar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Descargar   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Correcto despliegue y visualización de la pagina principal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualiza la solicitud </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Envio de comentarios al usuario </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borrado de la solicitud </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edita Registro de solicitud redireccionando al submenú Financiaminto y Oblicaciones </t>
   </si>
   <si>
     <t xml:space="preserve">Descarga de Solicitud </t>
@@ -436,85 +283,13 @@
     <t xml:space="preserve">Ingresar las Credenciales </t>
   </si>
   <si>
-    <t xml:space="preserve">Se ingreso correctamente con el usuario proporcionado por el desarrollador </t>
-  </si>
-  <si>
     <t xml:space="preserve">Ingresar </t>
   </si>
   <si>
     <t xml:space="preserve">Ingresar a la aplicacción </t>
   </si>
   <si>
-    <t>Se queda pensando al iniciar sesión / Colores de la pantalla principal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cumple con la funcion del botón "Agregar" haciendo el despliegue en los dos submenús (Detalle botón Agregar) </t>
-  </si>
-  <si>
-    <t>1. SRPU-167</t>
-  </si>
-  <si>
     <t>1. SRPU-169  SRPU-170</t>
-  </si>
-  <si>
-    <t>SRPU-173</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Permite Agregar y Eliminar Registros (Detalles Acentos, Mensajes de confirmación,  no tiene rango en número de pago , clear y no options en ingles.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRPU-174 /  SRPU-175 / SRPU-176 / SRPU-177 </t>
-  </si>
-  <si>
-    <t>SRPU-178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRPU-179 </t>
-  </si>
-  <si>
-    <t>SRPU-180</t>
-  </si>
-  <si>
-    <t>Botón Eliminar no tiene confirmación de borrado, Botón Agregar aparece del lago superior derecho de la pantalla
-Letras color azul
-sugerencia colocarlo en otra posición</t>
-  </si>
-  <si>
-    <t>File en ingles
-Sugerencia Archivos Considero Tener algún permiso para cargar los pdf ya que sube cualquier
-archivo sin importar que los nombres hagan match con el documento
-solicitado</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> La opción "BORRAR" solo se visualizara cuando este el archivo cargado?
-La opción "BORRAR" solo se visualizara cuando este el archivo cargado?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizacón correcta </t>
-  </si>
-  <si>
-    <t>Arroja Mensaje de error al darle clic en solicitar modificación Acento en la palabra modificación</t>
-  </si>
-  <si>
-    <t>SRPU-181  SRPU-182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No se visualizan las letras del botón confirmar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finaliza la solicitud y direcciona al apartado "Consulta de Solicitudes" </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edición Correcta (Descripción del tooltip botón Editar)
-faltan letras aparece Edit / Editar
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borra solicitudes / Detalles mensaje de confirmación </t>
-  </si>
-  <si>
-    <t>SRPU-186</t>
   </si>
   <si>
     <t>En Curso</t>
@@ -538,9 +313,6 @@
     <t xml:space="preserve">Administración de Plataformas </t>
   </si>
   <si>
-    <t>disrec</t>
-  </si>
-  <si>
     <t>PAUA</t>
   </si>
   <si>
@@ -554,6 +326,96 @@
   </si>
   <si>
     <t xml:space="preserve">Matriz de Pruebas PAUA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuarios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resgistrar Usuarios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizar Acceso a Plataforma </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columnas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtros </t>
+  </si>
+  <si>
+    <t>Densidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exportar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro de Usuarios </t>
+  </si>
+  <si>
+    <t>irisc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ortografía </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplicaciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro de Aplicación </t>
+  </si>
+  <si>
+    <t>Editar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar </t>
+  </si>
+  <si>
+    <t>Desnsidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicitides </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtro por aplicación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aceptar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechazar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ver comentarios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permiso Para Firmar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botón Siguiente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botón Anterior </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerrar Sesión </t>
+  </si>
+  <si>
+    <t>http://10.200.4.165/</t>
+  </si>
+  <si>
+    <t>Cierra sesión despues de dejar de usar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresar correctamente con la credencial asignada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajustar tooltip descriptivos </t>
+  </si>
+  <si>
+    <t>https://paua-sfytgenl.atlassian.net/browse/KPAUA-205</t>
   </si>
 </sst>
 </file>
@@ -2173,7 +2035,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2568,7 +2429,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2689,7 +2549,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3753,7 +3612,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5681,13 +5539,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1733107</xdr:colOff>
+          <xdr:colOff>1727348</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>380114</xdr:colOff>
+          <xdr:colOff>317205</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>200911</xdr:rowOff>
         </xdr:to>
@@ -5728,13 +5586,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>1733107</xdr:colOff>
+          <xdr:colOff>1727348</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>886</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>380114</xdr:colOff>
+          <xdr:colOff>317205</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>200911</xdr:rowOff>
         </xdr:to>
@@ -11673,7 +11531,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="A24:B27" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" showAll="0"/>
@@ -11750,7 +11608,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" showAll="0"/>
@@ -11859,7 +11717,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A47:E50" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -12348,7 +12206,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:N2"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12371,7 +12229,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -12405,7 +12263,7 @@
     </row>
     <row r="3" spans="1:14" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -12446,7 +12304,7 @@
       <c r="B5" s="24"/>
       <c r="C5" s="25"/>
       <c r="D5" s="35" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="E5" s="36"/>
       <c r="F5" s="37"/>
@@ -12508,77 +12366,75 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J7" s="21">
-        <v>85</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="J7" s="21"/>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L7" t="s">
-        <v>134</v>
-      </c>
-      <c r="M7" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="N7" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="M7" s="22"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="33" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
         <v>25</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="K8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L8" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="N8" s="1"/>
     </row>
@@ -12587,31 +12443,31 @@
         <v>3</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M9" s="22"/>
       <c r="N9" s="1"/>
@@ -12621,31 +12477,31 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M10" s="7"/>
       <c r="N10" s="1">
@@ -12657,435 +12513,304 @@
         <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="I11" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="M12" s="7"/>
-      <c r="N12" s="1">
-        <v>45071</v>
-      </c>
+      <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="I13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" t="s">
-        <v>132</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="N14" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="M14" s="7"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" t="s">
-        <v>134</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="N15" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="M15" s="7"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="G16" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K16" t="s">
-        <v>39</v>
-      </c>
-      <c r="L16" t="s">
-        <v>132</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N16" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="M16" s="7"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K17" t="s">
-        <v>39</v>
-      </c>
-      <c r="L17" t="s">
-        <v>132</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="N17" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="M17" s="7"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G18" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K18" t="s">
-        <v>39</v>
-      </c>
-      <c r="L18" t="s">
-        <v>132</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="N18" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="M18" s="7"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="J19" s="7"/>
-      <c r="K19" t="s">
-        <v>39</v>
-      </c>
       <c r="M19" s="7"/>
-      <c r="N19" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="J20" s="7"/>
-      <c r="K20" t="s">
-        <v>39</v>
-      </c>
       <c r="M20" s="7"/>
-      <c r="N20" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K21" t="s">
-        <v>39</v>
-      </c>
       <c r="M21" s="7"/>
-      <c r="N21" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>81</v>
@@ -13093,72 +12818,49 @@
       <c r="G22" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K22" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="N22" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="M22" s="7"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="K23" t="s">
-        <v>39</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="N23" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="M23" s="7"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>83</v>
@@ -13166,37 +12868,24 @@
       <c r="G24" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M24" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="N24" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="M24" s="7"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>84</v>
@@ -13204,40 +12893,24 @@
       <c r="G25" t="s">
         <v>27</v>
       </c>
-      <c r="H25" t="s">
-        <v>124</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" t="s">
-        <v>132</v>
-      </c>
-      <c r="M25" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="N25" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="M25" s="7"/>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>85</v>
@@ -13245,311 +12918,354 @@
       <c r="G26" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K26" t="s">
-        <v>39</v>
-      </c>
       <c r="M26" s="7"/>
-      <c r="N26" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="K27" t="s">
-        <v>39</v>
-      </c>
       <c r="M27" s="7"/>
-      <c r="N27" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K28" t="s">
-        <v>39</v>
-      </c>
       <c r="M28" s="7"/>
-      <c r="N28" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="G29" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K29" t="s">
-        <v>39</v>
-      </c>
       <c r="M29" s="7"/>
-      <c r="N29" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E30" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G30" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="K30" t="s">
-        <v>39</v>
-      </c>
       <c r="M30" s="7"/>
-      <c r="N30" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
         <v>25</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K31" t="s">
-        <v>39</v>
+        <v>99</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="N31" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>26</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="G32" t="s">
         <v>25</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K32" t="s">
-        <v>39</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N32" s="1">
-        <v>45071</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="33" x14ac:dyDescent="0.3">
+      <c r="M32" s="7"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="G33" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="K33" t="s">
-        <v>39</v>
-      </c>
-      <c r="N33" s="1">
-        <v>45071</v>
-      </c>
+      <c r="M33" s="7"/>
+      <c r="N33" s="1"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C34" s="3"/>
+      <c r="B34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B37"/>
-      <c r="F37"/>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" t="s">
+        <v>90</v>
+      </c>
       <c r="H37"/>
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B38"/>
-      <c r="F38"/>
+      <c r="B38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" t="s">
+        <v>91</v>
+      </c>
       <c r="H38"/>
       <c r="N38" s="1"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B39"/>
-      <c r="F39"/>
+      <c r="B39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" t="s">
+        <v>92</v>
+      </c>
       <c r="H39"/>
       <c r="N39" s="1"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B40"/>
-      <c r="F40"/>
+      <c r="B40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" t="s">
+        <v>93</v>
+      </c>
       <c r="H40"/>
       <c r="N40" s="1"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B41"/>
-      <c r="F41"/>
+      <c r="B41" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" t="s">
+        <v>94</v>
+      </c>
       <c r="H41"/>
       <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B42"/>
-      <c r="F42"/>
+      <c r="C42" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" t="s">
+        <v>95</v>
+      </c>
       <c r="H42"/>
       <c r="N42" s="1"/>
     </row>
@@ -14565,31 +14281,28 @@
     <mergeCell ref="G5:N5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="M7" r:id="rId1" display="https://srpu.atlassian.net/browse/SRPU-167"/>
-    <hyperlink ref="M14" r:id="rId2" display="https://srpu.atlassian.net/browse/SRPU-169"/>
-    <hyperlink ref="M15" r:id="rId3" display="https://srpu.atlassian.net/browse/SRPU-169"/>
-    <hyperlink ref="M17" r:id="rId4" display="https://srpu.atlassian.net/browse/SRPU-169"/>
-    <hyperlink ref="M16" r:id="rId5" display="https://srpu.atlassian.net/browse/SRPU-169"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="M31" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-  <drawing r:id="rId7"/>
-  <legacyDrawing r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3090" r:id="rId9" name="Control 18">
-          <controlPr defaultSize="0" r:id="rId10">
+        <control shapeId="3088" r:id="rId6" name="Control 16">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1733550</xdr:colOff>
+                <xdr:colOff>1724025</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>381000</xdr:colOff>
+                <xdr:colOff>314325</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>200025</xdr:rowOff>
               </to>
@@ -14598,23 +14311,23 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3090" r:id="rId9" name="Control 18"/>
+        <control shapeId="3088" r:id="rId6" name="Control 16"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3088" r:id="rId11" name="Control 16">
-          <controlPr defaultSize="0" r:id="rId10">
+        <control shapeId="3090" r:id="rId8" name="Control 18">
+          <controlPr defaultSize="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>1733550</xdr:colOff>
+                <xdr:colOff>1724025</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>381000</xdr:colOff>
+                <xdr:colOff>314325</xdr:colOff>
                 <xdr:row>9</xdr:row>
                 <xdr:rowOff>200025</xdr:rowOff>
               </to>
@@ -14623,12 +14336,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3088" r:id="rId11" name="Control 16"/>
+        <control shapeId="3090" r:id="rId8" name="Control 18"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -14637,7 +14350,7 @@
           <x14:formula1>
             <xm:f>Datos!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K55:K360 K34:K48</xm:sqref>
+          <xm:sqref>K55:K360 K12:K48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -14649,7 +14362,7 @@
           <x14:formula1>
             <xm:f>Datos!$D$2:$D$15</xm:f>
           </x14:formula1>
-          <xm:sqref>K7:K33</xm:sqref>
+          <xm:sqref>K7:K11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -14741,7 +14454,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="B25" s="12">
         <v>2</v>
@@ -14749,7 +14462,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="B26" s="16">
         <v>6</v>
@@ -14776,13 +14489,13 @@
         <v>18</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
@@ -14790,7 +14503,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="17"/>
       <c r="C49" s="17">
@@ -14856,7 +14569,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -14867,7 +14580,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -14878,7 +14591,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>28</v>
@@ -14886,60 +14599,60 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>